<commit_message>
Added Working Test Rail API, Tests show on UI
</commit_message>
<xml_diff>
--- a/clientTestData/CBIZ_09012021_Primary_09012021_{Automation}_{REGISTERED}.xlsx
+++ b/clientTestData/CBIZ_09012021_Primary_09012021_{Automation}_{REGISTERED}.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ulaxmira/Documents/RallyMochaFramework/clientTestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinay.marapaka/Documents/RallyMochaFramework/clientTestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C9D772-40C7-5145-9ECA-4903EC25D05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A6FA5F-1993-5243-BFB4-F1F5A5EA980C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="1060" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="10900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>CUST_ID</t>
   </si>
@@ -178,17 +178,28 @@
     <t>AkzoNobel Coatings, Inc</t>
   </si>
   <si>
-    <t>PROD_ANC_AUM_AFF1a@mailinator.com</t>
+    <t>abhinay.marapaka@rallyhealth.com</t>
+  </si>
+  <si>
+    <t>AbhinayElias22$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,10 +243,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,8 +264,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="W13" sqref="W13"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -721,11 +737,11 @@
       <c r="T2" s="3"/>
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="6" t="s">
         <v>52</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Comitting working changes will create another branch
</commit_message>
<xml_diff>
--- a/clientTestData/CBIZ_09012021_Primary_09012021_{Automation}_{REGISTERED}.xlsx
+++ b/clientTestData/CBIZ_09012021_Primary_09012021_{Automation}_{REGISTERED}.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinay.marapaka/Documents/RallyMochaFramework/clientTestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinay.marapaka/Desktop/RallyMochaFramework/clientTestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A6FA5F-1993-5243-BFB4-F1F5A5EA980C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842102F1-2822-4042-8D50-C85F26EECEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="10900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>CUST_ID</t>
   </si>
@@ -151,9 +151,6 @@
     <t>2021.09.01_CBIZ_Aff2_EREPR</t>
   </si>
   <si>
-    <t>uat_HJTfIdXh@rally.mailinator.com</t>
-  </si>
-  <si>
     <t>7fda1573-526a-4be9-a20c-a85b6759be27</t>
   </si>
   <si>
@@ -178,10 +175,10 @@
     <t>AkzoNobel Coatings, Inc</t>
   </si>
   <si>
-    <t>abhinay.marapaka@rallyhealth.com</t>
-  </si>
-  <si>
-    <t>AbhinayElias22$</t>
+    <t>RR2tprod@mailinator.com</t>
+  </si>
+  <si>
+    <t>RR1prodt@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -585,7 +582,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -709,7 +706,7 @@
         <v>28</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3">
         <v>3</v>
@@ -738,10 +735,10 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>35</v>
@@ -792,29 +789,29 @@
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
-      <c r="W3" s="3" t="s">
-        <v>43</v>
+      <c r="W3" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>34</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>29</v>
@@ -848,18 +845,19 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>34</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="W2" r:id="rId1" xr:uid="{3A62B193-AEB1-D247-8CEE-86F944E26918}"/>
+    <hyperlink ref="W3" r:id="rId2" xr:uid="{EAE97B78-55A2-3C46-B636-93DAF10ACCDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>